<commit_message>
finish 3/5-3/10 data cleaning
</commit_message>
<xml_diff>
--- a/data/xlsx/01142019.xlsx
+++ b/data/xlsx/01142019.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelli/Desktop/SUSA/[s19] web dev/susa-data-viz/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelli/Desktop/SUSA/[s19] web dev/susa-data-viz/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8A38B34-D433-6A44-8A59-73619321DA46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92E64893-2319-F641-8DCB-44873FF2CA80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="940" windowWidth="27000" windowHeight="16560" xr2:uid="{ABFC7FDC-9AAB-404E-8FC6-0F8FB5E25A94}"/>
+    <workbookView xWindow="2920" yWindow="940" windowWidth="10600" windowHeight="16560" xr2:uid="{ABFC7FDC-9AAB-404E-8FC6-0F8FB5E25A94}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="01142019" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -69,10 +69,6 @@
     <t>335 OHLONE AVE</t>
   </si>
   <si>
-    <t>(FA-33-O) REPORTS ATTEMPTED THEFT OF HER CATALYTIC CONVERTER ON HER RED 2006 HONDA ELEMENT, 7TVB326, 335 OHLONE AVE.
-SUSPECTS: MALE UNK RACE, 508, STOCKY BUILD, BLK HOODIE. RESPONSIBLE VEHICLE: DRK COLORED FORD EXPLORER.</t>
-  </si>
-  <si>
     <t>2:45</t>
   </si>
   <si>
@@ -97,10 +93,6 @@
     <t>MOFFITT LIBRARY</t>
   </si>
   <si>
-    <t>(MH-27-E) VICTIM OF HIT &amp; RUN, N/S MOFFITT LIBRARY SUSPECT: MB DRIVER
-VEHICLE: RED/WHITE CAMERO</t>
-  </si>
-  <si>
     <t>8:06</t>
   </si>
   <si>
@@ -258,6 +250,12 @@
   </si>
   <si>
     <t>DWINELLE HALL</t>
+  </si>
+  <si>
+    <t>(FA-33-O) REPORTS ATTEMPTED THEFT OF HER CATALYTIC CONVERTER ON HER RED 2006 HONDA ELEMENT, 7TVB326, 335 OHLONE AVE. SUSPECTS: MALE UNK RACE, 508, STOCKY BUILD, BLK HOODIE. RESPONSIBLE VEHICLE: DRK COLORED FORD EXPLORER.</t>
+  </si>
+  <si>
+    <t>(MH-27-E) VICTIM OF HIT &amp; RUN, N/S MOFFITT LIBRARY SUSPECT: MB DRIVER. VEHICLE: RED/WHITE CAMERO</t>
   </si>
 </sst>
 </file>
@@ -630,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D181A-F951-3D4B-9610-677D0322048A}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -643,7 +641,7 @@
     <col min="7" max="7" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,9 +666,8 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" ht="296">
+    </row>
+    <row r="2" spans="1:8" ht="296">
       <c r="A2" s="3">
         <v>43479</v>
       </c>
@@ -693,25 +690,24 @@
         <v>-122.30510700000001</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
       <c r="F3">
         <v>37.868876999999998</v>
@@ -720,25 +716,24 @@
         <v>-122.266302</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="121">
+      <c r="A4" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" ht="121">
-      <c r="A4" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>37.872793999999999</v>
@@ -747,25 +742,24 @@
         <v>-122.260716</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="F5">
         <v>37.868490000000001</v>
@@ -774,25 +768,24 @@
         <v>-122.261161</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3">
         <v>43479</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="F6">
         <v>37.872160000000001</v>
@@ -801,25 +794,24 @@
         <v>-122.266441</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="3">
         <v>43479</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7">
         <v>37.873652</v>
@@ -828,25 +820,24 @@
         <v>-122.259727</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="F8">
         <v>37.874039000000003</v>
@@ -855,25 +846,24 @@
         <v>-122.266457</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="F9">
         <v>37.871597999999999</v>
@@ -882,25 +872,24 @@
         <v>-122.26321</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="3">
         <v>43479</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F10">
         <v>37.86938</v>
@@ -909,25 +898,24 @@
         <v>-122.26058500000001</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="3">
         <v>43479</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="F11">
         <v>37.866520999999999</v>
@@ -936,25 +924,24 @@
         <v>-122.256304</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="3">
         <v>43479</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12">
         <v>37.869459999999997</v>
@@ -963,25 +950,24 @@
         <v>-122.259685</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="3">
         <v>43479</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13">
         <v>37.874039000000003</v>
@@ -990,25 +976,24 @@
         <v>-122.266457</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="3">
         <v>43479</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="F14">
         <v>37.867904000000003</v>
@@ -1017,47 +1002,44 @@
         <v>-122.266867</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="H15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="F16">
         <v>37.866947000000003</v>
@@ -1066,25 +1048,24 @@
         <v>-122.254817</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="3">
         <v>43479</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="F17">
         <v>37.874934000000003</v>
@@ -1093,25 +1074,24 @@
         <v>-122.255144</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="3">
         <v>43479</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F18">
         <v>37.866663000000003</v>
@@ -1120,25 +1100,24 @@
         <v>-122.260604</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="3">
         <v>43479</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="F19">
         <v>37.871383000000002</v>
@@ -1147,25 +1126,24 @@
         <v>-122.266711</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="3">
         <v>43479</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F20">
         <v>37.867904000000003</v>
@@ -1174,26 +1152,24 @@
         <v>-122.266867</v>
       </c>
       <c r="H20" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="3">
+        <v>43479</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="3">
-        <v>43479</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="F21">
         <v>37.870547000000002</v>
@@ -1202,9 +1178,8 @@
         <v>-122.260603</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="4"/>
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add jan and feb layers
</commit_message>
<xml_diff>
--- a/data/xlsx/01142019.xlsx
+++ b/data/xlsx/01142019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelli/Desktop/SUSA/[s19] web dev/susa-data-viz/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelli/Desktop/SUSA/susa-data-viz/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D675667B-E761-864F-B02F-7499BB4A9658}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E46411-9358-9849-86A9-D91A55BC7F2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="940" windowWidth="10600" windowHeight="16560" xr2:uid="{ABFC7FDC-9AAB-404E-8FC6-0F8FB5E25A94}"/>
+    <workbookView xWindow="2260" yWindow="1000" windowWidth="23040" windowHeight="16560" xr2:uid="{ABFC7FDC-9AAB-404E-8FC6-0F8FB5E25A94}"/>
   </bookViews>
   <sheets>
     <sheet name="01142019" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -193,15 +193,6 @@
   </si>
   <si>
     <t>TWO SUBJECTS CONTACTED FOR SUSPECTED PROWLING, BANWAY LOT.</t>
-  </si>
-  <si>
-    <t>19:33</t>
-  </si>
-  <si>
-    <t>VEHICLE CODE VIOLATION</t>
-  </si>
-  <si>
-    <t>CAMPUS</t>
   </si>
   <si>
     <t>19:47</t>
@@ -263,7 +254,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -316,7 +307,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D181A-F951-3D4B-9610-677D0322048A}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="89" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -693,7 +684,7 @@
         <v>-122.30510700000001</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -745,7 +736,7 @@
         <v>-122.260716</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1016,13 +1007,19 @@
         <v>54</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>56</v>
+      <c r="F15">
+        <v>37.866947000000003</v>
+      </c>
+      <c r="G15">
+        <v>-122.254817</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>15</v>
@@ -1033,22 +1030,22 @@
         <v>43479</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F16">
-        <v>37.866947000000003</v>
+        <v>37.874934000000003</v>
       </c>
       <c r="G16">
-        <v>-122.254817</v>
+        <v>-122.255144</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>15</v>
@@ -1062,19 +1059,19 @@
         <v>59</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="F17">
-        <v>37.874934000000003</v>
+        <v>37.866663000000003</v>
       </c>
       <c r="G17">
-        <v>-122.255144</v>
+        <v>-122.260604</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>15</v>
@@ -1085,22 +1082,22 @@
         <v>43479</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F18">
-        <v>37.866663000000003</v>
+        <v>37.871383000000002</v>
       </c>
       <c r="G18">
-        <v>-122.260604</v>
+        <v>-122.266711</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>15</v>
@@ -1111,25 +1108,25 @@
         <v>43479</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19">
+        <v>37.867904000000003</v>
+      </c>
+      <c r="G19">
+        <v>-122.266867</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="F19">
-        <v>37.871383000000002</v>
-      </c>
-      <c r="G19">
-        <v>-122.266711</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1140,47 +1137,21 @@
         <v>68</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F20">
-        <v>37.867904000000003</v>
+        <v>37.870547000000002</v>
       </c>
       <c r="G20">
-        <v>-122.266867</v>
+        <v>-122.260603</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="5">
-        <v>43479</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21">
-        <v>37.870547000000002</v>
-      </c>
-      <c r="G21">
-        <v>-122.260603</v>
-      </c>
-      <c r="H21" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>